<commit_message>
added username reset + integration with new phases process for security operations + changed jwtToken construction
</commit_message>
<xml_diff>
--- a/files/documentation/BackendTimeline.xlsx
+++ b/files/documentation/BackendTimeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22534C2-B0A5-4B79-BDA2-22E95FFF96B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB8E8BA8-F9A0-4314-86BA-13CFE73BD225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-7290" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Day</t>
   </si>
@@ -197,6 +197,9 @@
   </si>
   <si>
     <t xml:space="preserve">Made swagger with auth header, password reset with security code </t>
+  </si>
+  <si>
+    <t>Changed User Protected Details update with process phases for better FE controll</t>
   </si>
 </sst>
 </file>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D41"/>
+  <dimension ref="A2:D42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -1038,27 +1041,41 @@
         <v>58</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
-      <c r="C39" s="4" t="s">
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>30</v>
+      </c>
+      <c r="B38" s="2">
+        <v>45570</v>
+      </c>
+      <c r="C38" s="1">
+        <v>5</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="C40" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="4">
+      <c r="D40" s="4">
         <f>SUM(C4:C38)</f>
-        <v>148.81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
-      <c r="C40" s="5"/>
-      <c r="D40" s="4"/>
+        <v>153.81</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="C41" s="5"/>
       <c r="D41" s="4"/>
     </row>
+    <row r="42" spans="1:4">
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="C40:C42"/>
+    <mergeCell ref="D40:D42"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
made sinopsis + multumiri documentatie
</commit_message>
<xml_diff>
--- a/files/documentation/BackendTimeline.xlsx
+++ b/files/documentation/BackendTimeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ALEX PROGRAMARE\SwapIt\files\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0387191-9BA6-4F15-A10A-7E9A55ED35F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2792BA3-6367-41E5-B07A-9365918D7A26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -553,8 +553,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4"/>

</xml_diff>